<commit_message>
updated questions on 220905
Added new questions to the questions tab of results.xlsx regarding how to set big M
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B05E6B-05C4-7E43-A391-836C9CE02055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32200" windowHeight="19780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
     <sheet name="questions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Stage1</t>
   </si>
@@ -104,12 +116,21 @@
   </si>
   <si>
     <t>Any reference regarding the value of M?</t>
+  </si>
+  <si>
+    <t>should we use a different value of M for each candidate line?</t>
+  </si>
+  <si>
+    <t>M &lt;- Psk/max(deltaTheta)*xsk; max(deltaTheta) = pi/4</t>
+  </si>
+  <si>
+    <t>if we use the same M for all candidate lines, should we use the Max(Psk) and min(xsk) or some other combination of values?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,12 +210,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,21 +495,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.1796875" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" customWidth="1"/>
-    <col min="5" max="5" width="26.54296875" customWidth="1"/>
+    <col min="1" max="1" width="38.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -519,7 +540,7 @@
         <v>5406.98</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -539,7 +560,7 @@
         <v>1.657128246008517</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -550,7 +571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>0</v>
       </c>
@@ -558,7 +579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>0</v>
       </c>
@@ -566,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>1</v>
       </c>
@@ -574,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>1</v>
       </c>
@@ -582,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>0</v>
       </c>
@@ -590,7 +611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -607,7 +628,7 @@
         <v>61.343555707662397</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>0</v>
       </c>
@@ -621,7 +642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>0</v>
       </c>
@@ -635,7 +656,7 @@
         <v>22.461228840785399</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>100</v>
       </c>
@@ -649,7 +670,7 @@
         <v>99.999999999996902</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>38.033809365493802</v>
       </c>
@@ -663,7 +684,7 @@
         <v>32.256125850940997</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>0</v>
       </c>
@@ -677,17 +698,17 @@
         <v>-29.1764613890197</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B20" s="7" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -701,7 +722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
@@ -718,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>9</v>
       </c>
@@ -735,7 +756,7 @@
         <v>35.635125381009402</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>1</v>
       </c>
@@ -749,7 +770,7 @@
         <v>-36.135181200710797</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>0</v>
       </c>
@@ -763,7 +784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>1</v>
       </c>
@@ -777,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>1</v>
       </c>
@@ -791,7 +812,7 @@
         <v>-30.045836396229799</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>0</v>
       </c>
@@ -805,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>1</v>
       </c>
@@ -819,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>0</v>
       </c>
@@ -833,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>1</v>
       </c>
@@ -847,7 +868,7 @@
         <v>13.761720136141401</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>7</v>
       </c>
@@ -864,7 +885,7 @@
         <v>-83.359019403107396</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>9</v>
       </c>
@@ -881,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>0</v>
       </c>
@@ -895,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>0</v>
       </c>
@@ -909,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>0</v>
       </c>
@@ -923,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>1</v>
       </c>
@@ -937,7 +958,7 @@
         <v>-31.621466065322501</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>1</v>
       </c>
@@ -951,7 +972,7 @@
         <v>-31.463121217724499</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B40">
         <v>0</v>
       </c>
@@ -965,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>0</v>
       </c>
@@ -979,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>1</v>
       </c>
@@ -993,7 +1014,7 @@
         <v>-32.673870552155897</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>1</v>
       </c>
@@ -1007,7 +1028,7 @@
         <v>-47.730506204577303</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>0</v>
       </c>
@@ -1021,7 +1042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>0</v>
       </c>
@@ -1035,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>0</v>
       </c>
@@ -1049,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>0</v>
       </c>
@@ -1063,7 +1084,7 @@
         <v>19.0862251129392</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>0</v>
       </c>
@@ -1077,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>0</v>
       </c>
@@ -1091,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B50">
         <v>0</v>
       </c>
@@ -1105,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>8</v>
       </c>
@@ -1122,7 +1143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>9</v>
       </c>
@@ -1139,11 +1160,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="9"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="8"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>14</v>
       </c>
@@ -1157,8 +1178,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="10" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B57">
@@ -1174,7 +1195,7 @@
         <v>23.2710566932546</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B58">
         <v>19.0862251129392</v>
       </c>
@@ -1188,7 +1209,7 @@
         <v>-3.7390592906257302E-6</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B59">
         <v>-30.2076216691326</v>
       </c>
@@ -1202,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>11.300692998524401</v>
       </c>
@@ -1216,7 +1237,7 @@
         <v>-7.93144262868362E-6</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B61">
         <v>100</v>
       </c>
@@ -1230,7 +1251,7 @@
         <v>40.023558095881</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B62">
         <v>31.415926535897899</v>
       </c>
@@ -1244,7 +1265,7 @@
         <v>22.007578444928299</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B63">
         <v>57.119866428905297</v>
       </c>
@@ -1258,7 +1279,7 @@
         <v>2.5634507233769201E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B64">
         <v>-30.2076216691326</v>
       </c>
@@ -1272,28 +1293,28 @@
         <v>-18.913320409440299</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B67" s="7" t="s">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B67" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7" t="s">
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
-      <c r="I67" s="7"/>
-      <c r="J67" s="7" t="s">
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K67" s="7"/>
-      <c r="L67" s="7"/>
-      <c r="M67" s="7"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A68" s="8" t="s">
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A68" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B68" t="s">
@@ -1333,7 +1354,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B69">
         <v>135.728943306742</v>
       </c>
@@ -1371,7 +1392,7 @@
         <v>1.03883252437184E-11</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B70" s="6">
         <v>0</v>
       </c>
@@ -1409,7 +1430,7 @@
         <v>4.4240436340890402E-12</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B71">
         <v>0</v>
       </c>
@@ -1447,7 +1468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B72">
         <v>0</v>
       </c>
@@ -1485,7 +1506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B73">
         <v>0</v>
       </c>
@@ -1523,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B74">
         <v>0</v>
       </c>
@@ -1549,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B75">
         <v>0</v>
       </c>
@@ -1575,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B76">
         <v>0</v>
       </c>
@@ -1601,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B77">
         <v>0</v>
       </c>
@@ -1627,7 +1648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B78">
         <v>0</v>
       </c>
@@ -1653,7 +1674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B79">
         <v>0</v>
       </c>
@@ -1679,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B80">
         <v>0</v>
       </c>
@@ -1705,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81">
         <v>0</v>
       </c>
@@ -1731,7 +1752,7 @@
         <v>39.9999999998386</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B82">
         <v>0</v>
       </c>
@@ -1757,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F83">
         <v>0</v>
       </c>
@@ -1771,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F84">
         <v>0</v>
       </c>
@@ -1785,7 +1806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F85">
         <v>0</v>
       </c>
@@ -1799,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F86">
         <v>0</v>
       </c>
@@ -1813,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F87">
         <v>0</v>
       </c>
@@ -1827,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F88">
         <v>0</v>
       </c>
@@ -1841,7 +1862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F89">
         <v>0</v>
       </c>
@@ -1855,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F90">
         <v>37.014152928694003</v>
       </c>
@@ -1869,7 +1890,7 @@
         <v>25.7196279757807</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F91">
         <v>0</v>
       </c>
@@ -1883,7 +1904,7 @@
         <v>1.07537816502064E-10</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F92">
         <v>0</v>
       </c>
@@ -1897,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F93">
         <v>0</v>
       </c>
@@ -1911,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F94">
         <v>0</v>
       </c>
@@ -1925,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F95">
         <v>0</v>
       </c>
@@ -1939,7 +1960,7 @@
         <v>2.0813770895022899E-11</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F96">
         <v>0</v>
       </c>
@@ -1953,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="6:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F97">
         <v>0</v>
       </c>
@@ -1967,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="6:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F98">
         <v>0</v>
       </c>
@@ -1994,19 +2015,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="111.6328125" customWidth="1"/>
+    <col min="2" max="2" width="111.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2014,7 +2035,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2022,7 +2043,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2030,7 +2051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2038,12 +2059,31 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>